<commit_message>
finalized log regression and tested k-means generalization
</commit_message>
<xml_diff>
--- a/expanded_data/testing.xlsx
+++ b/expanded_data/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bushi\Desktop\University\Year 3\Courses\MIE368\MIE368-UFC\expanded_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8BCE85-C0DD-40E2-977D-C81575B84434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335BCAEE-2171-44EB-9BAC-C8E95795C761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>M_NAME</t>
   </si>
@@ -178,6 +178,51 @@
   </si>
   <si>
     <t>Jon Jones</t>
+  </si>
+  <si>
+    <t>Kron Gracie</t>
+  </si>
+  <si>
+    <t>Luke Rockhold</t>
+  </si>
+  <si>
+    <t>Lyoto Machida</t>
+  </si>
+  <si>
+    <t>Matt Hughes</t>
+  </si>
+  <si>
+    <t>Matt Serra</t>
+  </si>
+  <si>
+    <t>Mauricio Rua</t>
+  </si>
+  <si>
+    <t>Nick Diaz</t>
+  </si>
+  <si>
+    <t>Ovince Saint Preux</t>
+  </si>
+  <si>
+    <t>Paul Felder</t>
+  </si>
+  <si>
+    <t>Michael Bisping</t>
+  </si>
+  <si>
+    <t>Quinton Jackson</t>
+  </si>
+  <si>
+    <t>Randy Couture</t>
+  </si>
+  <si>
+    <t>Rashad Evans</t>
+  </si>
+  <si>
+    <t>Rory MacDonald</t>
+  </si>
+  <si>
+    <t>Royce Gracie</t>
   </si>
 </sst>
 </file>
@@ -495,13 +540,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ16"/>
+  <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1:AI1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:AJ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2260,6 +2308,1656 @@
         <v>0.238095238095238</v>
       </c>
       <c r="AJ16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>3.3428571429999998</v>
+      </c>
+      <c r="E17">
+        <v>4.3476190480000003</v>
+      </c>
+      <c r="F17">
+        <v>0.23809523799999999</v>
+      </c>
+      <c r="G17">
+        <v>0.23809523799999999</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0.65</v>
+      </c>
+      <c r="J17">
+        <v>2.6714285709999999</v>
+      </c>
+      <c r="K17">
+        <v>0.133333333</v>
+      </c>
+      <c r="L17">
+        <v>0.53809523800000003</v>
+      </c>
+      <c r="M17">
+        <v>2.9428571429999999</v>
+      </c>
+      <c r="N17">
+        <v>0.366666667</v>
+      </c>
+      <c r="O17">
+        <v>3.3333333E-2</v>
+      </c>
+      <c r="P17">
+        <v>3.3333333E-2</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>5.4523809520000004</v>
+      </c>
+      <c r="S17">
+        <v>5.7190476190000004</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0.3</v>
+      </c>
+      <c r="X17">
+        <v>3.5142857140000001</v>
+      </c>
+      <c r="Y17">
+        <v>1.3333333329999999</v>
+      </c>
+      <c r="Z17">
+        <v>0.60476190500000004</v>
+      </c>
+      <c r="AA17">
+        <v>4.6190476189999998</v>
+      </c>
+      <c r="AB17">
+        <v>0.8</v>
+      </c>
+      <c r="AC17">
+        <v>3.3333333E-2</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0.5</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0.5</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>0.764705882</v>
+      </c>
+      <c r="C18">
+        <v>0.25332623799999998</v>
+      </c>
+      <c r="D18">
+        <v>6.0087449670000002</v>
+      </c>
+      <c r="E18">
+        <v>7.7218010619999999</v>
+      </c>
+      <c r="F18">
+        <v>2.9594782E-2</v>
+      </c>
+      <c r="G18">
+        <v>0.23879050499999999</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>2.0023809520000002</v>
+      </c>
+      <c r="J18">
+        <v>4.1520176800000002</v>
+      </c>
+      <c r="K18">
+        <v>1.3457101899999999</v>
+      </c>
+      <c r="L18">
+        <v>0.51101709699999998</v>
+      </c>
+      <c r="M18">
+        <v>2.0852947749999999</v>
+      </c>
+      <c r="N18">
+        <v>0.53295362000000002</v>
+      </c>
+      <c r="O18">
+        <v>3.390496572</v>
+      </c>
+      <c r="P18">
+        <v>5.3390371999999998E-2</v>
+      </c>
+      <c r="Q18">
+        <v>6.9730240999999998E-2</v>
+      </c>
+      <c r="R18">
+        <v>2.356196663</v>
+      </c>
+      <c r="S18">
+        <v>3.1335611939999999</v>
+      </c>
+      <c r="T18">
+        <v>8.0337512999999999E-2</v>
+      </c>
+      <c r="U18">
+        <v>1.8975332000000001E-2</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>1.503571429</v>
+      </c>
+      <c r="X18">
+        <v>1.2790058799999999</v>
+      </c>
+      <c r="Y18">
+        <v>0.42624159499999997</v>
+      </c>
+      <c r="Z18">
+        <v>0.65094918800000001</v>
+      </c>
+      <c r="AA18">
+        <v>1.7507960490000001</v>
+      </c>
+      <c r="AB18">
+        <v>0.378878622</v>
+      </c>
+      <c r="AC18">
+        <v>0.226521993</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0.117647059</v>
+      </c>
+      <c r="AH18">
+        <v>0.52941176499999998</v>
+      </c>
+      <c r="AI18">
+        <v>0.35294117600000002</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="C19">
+        <v>0.117138293</v>
+      </c>
+      <c r="D19">
+        <v>2.8959889350000001</v>
+      </c>
+      <c r="E19">
+        <v>3.5870742870000001</v>
+      </c>
+      <c r="F19">
+        <v>6.6644888999999999E-2</v>
+      </c>
+      <c r="G19">
+        <v>3.0654761999999999E-2</v>
+      </c>
+      <c r="H19">
+        <v>7.242063E-3</v>
+      </c>
+      <c r="I19">
+        <v>1.861805556</v>
+      </c>
+      <c r="J19">
+        <v>1.634678724</v>
+      </c>
+      <c r="K19">
+        <v>0.69364867200000002</v>
+      </c>
+      <c r="L19">
+        <v>0.56766153900000005</v>
+      </c>
+      <c r="M19">
+        <v>1.8995581640000001</v>
+      </c>
+      <c r="N19">
+        <v>0.34230048099999999</v>
+      </c>
+      <c r="O19">
+        <v>0.65413029</v>
+      </c>
+      <c r="P19">
+        <v>4.9058655999999999E-2</v>
+      </c>
+      <c r="Q19">
+        <v>3.2711535E-2</v>
+      </c>
+      <c r="R19">
+        <v>1.5554030480000001</v>
+      </c>
+      <c r="S19">
+        <v>2.542430226</v>
+      </c>
+      <c r="T19">
+        <v>5.5248209E-2</v>
+      </c>
+      <c r="U19">
+        <v>2.9987562999999998E-2</v>
+      </c>
+      <c r="V19">
+        <v>1.6666669999999999E-3</v>
+      </c>
+      <c r="W19">
+        <v>1.122222222</v>
+      </c>
+      <c r="X19">
+        <v>0.77444679599999999</v>
+      </c>
+      <c r="Y19">
+        <v>0.29100336599999999</v>
+      </c>
+      <c r="Z19">
+        <v>0.489952887</v>
+      </c>
+      <c r="AA19">
+        <v>0.95493512999999997</v>
+      </c>
+      <c r="AB19">
+        <v>0.310519726</v>
+      </c>
+      <c r="AC19">
+        <v>0.28994819199999999</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0.125</v>
+      </c>
+      <c r="AG19">
+        <v>0.33333333300000001</v>
+      </c>
+      <c r="AH19">
+        <v>0.41666666699999999</v>
+      </c>
+      <c r="AI19">
+        <v>0.125</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>0.72</v>
+      </c>
+      <c r="C20">
+        <v>1.7762238E-2</v>
+      </c>
+      <c r="D20">
+        <v>2.6134659490000001</v>
+      </c>
+      <c r="E20">
+        <v>3.9627033599999999</v>
+      </c>
+      <c r="F20">
+        <v>0.307324504</v>
+      </c>
+      <c r="G20">
+        <v>0.11096584600000001</v>
+      </c>
+      <c r="H20">
+        <v>2.5385662E-2</v>
+      </c>
+      <c r="I20">
+        <v>4.9083333329999999</v>
+      </c>
+      <c r="J20">
+        <v>1.664989552</v>
+      </c>
+      <c r="K20">
+        <v>0.74215751399999996</v>
+      </c>
+      <c r="L20">
+        <v>0.20631888300000001</v>
+      </c>
+      <c r="M20">
+        <v>0.93995815100000002</v>
+      </c>
+      <c r="N20">
+        <v>0.18102436699999999</v>
+      </c>
+      <c r="O20">
+        <v>1.4924834309999999</v>
+      </c>
+      <c r="P20">
+        <v>0.26781862499999998</v>
+      </c>
+      <c r="Q20">
+        <v>0.14806583300000001</v>
+      </c>
+      <c r="R20">
+        <v>2.3007941430000001</v>
+      </c>
+      <c r="S20">
+        <v>4.1611353979999999</v>
+      </c>
+      <c r="T20">
+        <v>5.0734645000000002E-2</v>
+      </c>
+      <c r="U20">
+        <v>0.19782149199999999</v>
+      </c>
+      <c r="V20">
+        <v>3.3022609000000001E-2</v>
+      </c>
+      <c r="W20">
+        <v>1.235416667</v>
+      </c>
+      <c r="X20">
+        <v>1.817728832</v>
+      </c>
+      <c r="Y20">
+        <v>0.31425041999999997</v>
+      </c>
+      <c r="Z20">
+        <v>0.16881489099999999</v>
+      </c>
+      <c r="AA20">
+        <v>1.168152275</v>
+      </c>
+      <c r="AB20">
+        <v>0.27847387400000001</v>
+      </c>
+      <c r="AC20">
+        <v>0.85416799300000001</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0.2</v>
+      </c>
+      <c r="AH20">
+        <v>0.4</v>
+      </c>
+      <c r="AI20">
+        <v>0.32</v>
+      </c>
+      <c r="AJ20">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21">
+        <v>8.1305686000000002E-2</v>
+      </c>
+      <c r="D21">
+        <v>2.257895752</v>
+      </c>
+      <c r="E21">
+        <v>4.0846343479999998</v>
+      </c>
+      <c r="F21">
+        <v>0.128935151</v>
+      </c>
+      <c r="G21">
+        <v>0.10570877300000001</v>
+      </c>
+      <c r="H21">
+        <v>2.3857624000000001E-2</v>
+      </c>
+      <c r="I21">
+        <v>4.1178571430000002</v>
+      </c>
+      <c r="J21">
+        <v>1.2420497189999999</v>
+      </c>
+      <c r="K21">
+        <v>0.66005006700000002</v>
+      </c>
+      <c r="L21">
+        <v>0.35579596600000002</v>
+      </c>
+      <c r="M21">
+        <v>1.359763091</v>
+      </c>
+      <c r="N21">
+        <v>0.283660784</v>
+      </c>
+      <c r="O21">
+        <v>0.61447187599999997</v>
+      </c>
+      <c r="P21">
+        <v>3.5945536E-2</v>
+      </c>
+      <c r="Q21">
+        <v>9.62001E-3</v>
+      </c>
+      <c r="R21">
+        <v>2.4709566860000001</v>
+      </c>
+      <c r="S21">
+        <v>5.6762630730000003</v>
+      </c>
+      <c r="T21">
+        <v>0.100828801</v>
+      </c>
+      <c r="U21">
+        <v>2.3809523999999999E-2</v>
+      </c>
+      <c r="V21">
+        <v>2.8667629E-2</v>
+      </c>
+      <c r="W21">
+        <v>2.526190476</v>
+      </c>
+      <c r="X21">
+        <v>1.636992547</v>
+      </c>
+      <c r="Y21">
+        <v>0.64424464400000003</v>
+      </c>
+      <c r="Z21">
+        <v>0.18971949499999999</v>
+      </c>
+      <c r="AA21">
+        <v>1.488520603</v>
+      </c>
+      <c r="AB21">
+        <v>0.43875013899999998</v>
+      </c>
+      <c r="AC21">
+        <v>0.54368594400000003</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>7.1428570999999996E-2</v>
+      </c>
+      <c r="AF21">
+        <v>0.14285714299999999</v>
+      </c>
+      <c r="AG21">
+        <v>0.428571429</v>
+      </c>
+      <c r="AH21">
+        <v>0.28571428599999998</v>
+      </c>
+      <c r="AI21">
+        <v>7.1428570999999996E-2</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C22">
+        <v>0.13789558800000001</v>
+      </c>
+      <c r="D22">
+        <v>3.9692022009999999</v>
+      </c>
+      <c r="E22">
+        <v>5.359993051</v>
+      </c>
+      <c r="F22">
+        <v>8.4927469000000005E-2</v>
+      </c>
+      <c r="G22">
+        <v>1.2182648000000001E-2</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>2.5691666670000002</v>
+      </c>
+      <c r="J22">
+        <v>2.364812192</v>
+      </c>
+      <c r="K22">
+        <v>0.54615190700000005</v>
+      </c>
+      <c r="L22">
+        <v>1.058238102</v>
+      </c>
+      <c r="M22">
+        <v>2.7802768979999999</v>
+      </c>
+      <c r="N22">
+        <v>0.432082311</v>
+      </c>
+      <c r="O22">
+        <v>0.75684299200000005</v>
+      </c>
+      <c r="P22">
+        <v>0.15142383100000001</v>
+      </c>
+      <c r="Q22">
+        <v>0.13224770499999999</v>
+      </c>
+      <c r="R22">
+        <v>4.2716517060000001</v>
+      </c>
+      <c r="S22">
+        <v>6.0412961010000004</v>
+      </c>
+      <c r="T22">
+        <v>0.14059252899999999</v>
+      </c>
+      <c r="U22">
+        <v>4.3685344000000001E-2</v>
+      </c>
+      <c r="V22">
+        <v>1.0779660999999999E-2</v>
+      </c>
+      <c r="W22">
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="X22">
+        <v>3.3466209139999998</v>
+      </c>
+      <c r="Y22">
+        <v>0.58804836500000002</v>
+      </c>
+      <c r="Z22">
+        <v>0.33698242699999997</v>
+      </c>
+      <c r="AA22">
+        <v>2.6874278450000002</v>
+      </c>
+      <c r="AB22">
+        <v>0.44625366</v>
+      </c>
+      <c r="AC22">
+        <v>1.1379702</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0.1</v>
+      </c>
+      <c r="AG22">
+        <v>0.2</v>
+      </c>
+      <c r="AH22">
+        <v>0.6</v>
+      </c>
+      <c r="AI22">
+        <v>0.1</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>0.7</v>
+      </c>
+      <c r="C23">
+        <v>0.10356578</v>
+      </c>
+      <c r="D23">
+        <v>6.5308729220000004</v>
+      </c>
+      <c r="E23">
+        <v>12.08889553</v>
+      </c>
+      <c r="F23">
+        <v>0.10214205799999999</v>
+      </c>
+      <c r="G23">
+        <v>9.0771128000000006E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.6711409E-2</v>
+      </c>
+      <c r="I23">
+        <v>1.984210526</v>
+      </c>
+      <c r="J23">
+        <v>4.7379920520000001</v>
+      </c>
+      <c r="K23">
+        <v>1.2037233570000001</v>
+      </c>
+      <c r="L23">
+        <v>0.58915751400000005</v>
+      </c>
+      <c r="M23">
+        <v>4.5448189589999997</v>
+      </c>
+      <c r="N23">
+        <v>1.3919319400000001</v>
+      </c>
+      <c r="O23">
+        <v>0.59412202199999997</v>
+      </c>
+      <c r="P23">
+        <v>1.7333332999999999E-2</v>
+      </c>
+      <c r="Q23">
+        <v>2.0892377E-2</v>
+      </c>
+      <c r="R23">
+        <v>2.9882176779999998</v>
+      </c>
+      <c r="S23">
+        <v>4.8072914659999997</v>
+      </c>
+      <c r="T23">
+        <v>9.4031012999999997E-2</v>
+      </c>
+      <c r="U23">
+        <v>3.1473314000000002E-2</v>
+      </c>
+      <c r="V23">
+        <v>1.8650164E-2</v>
+      </c>
+      <c r="W23">
+        <v>2.8333333330000001</v>
+      </c>
+      <c r="X23">
+        <v>1.9920467319999999</v>
+      </c>
+      <c r="Y23">
+        <v>0.56513341900000003</v>
+      </c>
+      <c r="Z23">
+        <v>0.43103752699999998</v>
+      </c>
+      <c r="AA23">
+        <v>2.0853263599999998</v>
+      </c>
+      <c r="AB23">
+        <v>0.50160229000000001</v>
+      </c>
+      <c r="AC23">
+        <v>0.40128902799999999</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0.05</v>
+      </c>
+      <c r="AG23">
+        <v>0.35</v>
+      </c>
+      <c r="AH23">
+        <v>0.35</v>
+      </c>
+      <c r="AI23">
+        <v>0.25</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>0.64285714299999996</v>
+      </c>
+      <c r="C24">
+        <v>9.1414869999999995E-2</v>
+      </c>
+      <c r="D24">
+        <v>3.227193405</v>
+      </c>
+      <c r="E24">
+        <v>4.4959039409999999</v>
+      </c>
+      <c r="F24">
+        <v>9.8455381999999994E-2</v>
+      </c>
+      <c r="G24">
+        <v>8.2331219999999997E-2</v>
+      </c>
+      <c r="H24">
+        <v>1.2236287E-2</v>
+      </c>
+      <c r="I24">
+        <v>1.649333333</v>
+      </c>
+      <c r="J24">
+        <v>2.4000524479999998</v>
+      </c>
+      <c r="K24">
+        <v>0.64203844099999996</v>
+      </c>
+      <c r="L24">
+        <v>0.185102515</v>
+      </c>
+      <c r="M24">
+        <v>1.6952675290000001</v>
+      </c>
+      <c r="N24">
+        <v>0.20532471099999999</v>
+      </c>
+      <c r="O24">
+        <v>1.326601165</v>
+      </c>
+      <c r="P24">
+        <v>3.3932558000000002E-2</v>
+      </c>
+      <c r="Q24">
+        <v>2.8773447000000001E-2</v>
+      </c>
+      <c r="R24">
+        <v>2.9898996690000001</v>
+      </c>
+      <c r="S24">
+        <v>4.3290108900000002</v>
+      </c>
+      <c r="T24">
+        <v>7.9078336999999999E-2</v>
+      </c>
+      <c r="U24">
+        <v>6.9061681999999999E-2</v>
+      </c>
+      <c r="V24">
+        <v>2.380952E-3</v>
+      </c>
+      <c r="W24">
+        <v>2.5739999999999998</v>
+      </c>
+      <c r="X24">
+        <v>1.4863219190000001</v>
+      </c>
+      <c r="Y24">
+        <v>0.69777704699999998</v>
+      </c>
+      <c r="Z24">
+        <v>0.80580070199999998</v>
+      </c>
+      <c r="AA24">
+        <v>1.994060309</v>
+      </c>
+      <c r="AB24">
+        <v>0.627740085</v>
+      </c>
+      <c r="AC24">
+        <v>0.368099275</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>3.5714285999999998E-2</v>
+      </c>
+      <c r="AF24">
+        <v>7.1428570999999996E-2</v>
+      </c>
+      <c r="AG24">
+        <v>0.28571428599999998</v>
+      </c>
+      <c r="AH24">
+        <v>0.321428571</v>
+      </c>
+      <c r="AI24">
+        <v>0.28571428599999998</v>
+      </c>
+      <c r="AJ24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>0.64285714299999996</v>
+      </c>
+      <c r="C25">
+        <v>4.3163736000000001E-2</v>
+      </c>
+      <c r="D25">
+        <v>3.818790806</v>
+      </c>
+      <c r="E25">
+        <v>4.5572597860000004</v>
+      </c>
+      <c r="F25">
+        <v>1.501481E-2</v>
+      </c>
+      <c r="G25">
+        <v>1.5379357E-2</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>1.707142857</v>
+      </c>
+      <c r="J25">
+        <v>2.196653408</v>
+      </c>
+      <c r="K25">
+        <v>0.76496325099999996</v>
+      </c>
+      <c r="L25">
+        <v>0.85717414800000002</v>
+      </c>
+      <c r="M25">
+        <v>2.5782291559999999</v>
+      </c>
+      <c r="N25">
+        <v>0.534178916</v>
+      </c>
+      <c r="O25">
+        <v>0.70638273500000004</v>
+      </c>
+      <c r="P25">
+        <v>2.2895493999999999E-2</v>
+      </c>
+      <c r="Q25">
+        <v>4.7619050000000003E-3</v>
+      </c>
+      <c r="R25">
+        <v>3.160905573</v>
+      </c>
+      <c r="S25">
+        <v>3.8515706559999998</v>
+      </c>
+      <c r="T25">
+        <v>0.101592486</v>
+      </c>
+      <c r="U25">
+        <v>1.5698587E-2</v>
+      </c>
+      <c r="V25">
+        <v>1.2611198000000001E-2</v>
+      </c>
+      <c r="W25">
+        <v>2.7059523809999999</v>
+      </c>
+      <c r="X25">
+        <v>1.5255053759999999</v>
+      </c>
+      <c r="Y25">
+        <v>0.81158094800000002</v>
+      </c>
+      <c r="Z25">
+        <v>0.82381924900000003</v>
+      </c>
+      <c r="AA25">
+        <v>2.7094786470000001</v>
+      </c>
+      <c r="AB25">
+        <v>0.31136251300000001</v>
+      </c>
+      <c r="AC25">
+        <v>0.140064413</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0.35714285699999998</v>
+      </c>
+      <c r="AG25">
+        <v>0.21428571399999999</v>
+      </c>
+      <c r="AH25">
+        <v>0.28571428599999998</v>
+      </c>
+      <c r="AI25">
+        <v>7.1428570999999996E-2</v>
+      </c>
+      <c r="AJ25">
+        <v>7.1428570999999996E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26">
+        <v>0.68965517200000004</v>
+      </c>
+      <c r="C26">
+        <v>4.2061569E-2</v>
+      </c>
+      <c r="D26">
+        <v>4.4424090080000003</v>
+      </c>
+      <c r="E26">
+        <v>5.6585580369999997</v>
+      </c>
+      <c r="F26">
+        <v>9.4632819000000007E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.8606758000000001E-2</v>
+      </c>
+      <c r="H26">
+        <v>1.3009404E-2</v>
+      </c>
+      <c r="I26">
+        <v>1.1454022989999999</v>
+      </c>
+      <c r="J26">
+        <v>3.193217733</v>
+      </c>
+      <c r="K26">
+        <v>0.64354935700000004</v>
+      </c>
+      <c r="L26">
+        <v>0.605641918</v>
+      </c>
+      <c r="M26">
+        <v>3.187211086</v>
+      </c>
+      <c r="N26">
+        <v>0.57991958399999999</v>
+      </c>
+      <c r="O26">
+        <v>0.67527833800000003</v>
+      </c>
+      <c r="P26">
+        <v>3.9745892999999997E-2</v>
+      </c>
+      <c r="Q26">
+        <v>4.9046456000000002E-2</v>
+      </c>
+      <c r="R26">
+        <v>2.6472295749999999</v>
+      </c>
+      <c r="S26">
+        <v>3.3890537479999998</v>
+      </c>
+      <c r="T26">
+        <v>9.8072516999999998E-2</v>
+      </c>
+      <c r="U26">
+        <v>4.3407042999999999E-2</v>
+      </c>
+      <c r="V26">
+        <v>6.0334450000000001E-3</v>
+      </c>
+      <c r="W26">
+        <v>1.896551724</v>
+      </c>
+      <c r="X26">
+        <v>1.490815124</v>
+      </c>
+      <c r="Y26">
+        <v>0.58224868799999996</v>
+      </c>
+      <c r="Z26">
+        <v>0.574165763</v>
+      </c>
+      <c r="AA26">
+        <v>2.1068825210000002</v>
+      </c>
+      <c r="AB26">
+        <v>0.24452795399999999</v>
+      </c>
+      <c r="AC26">
+        <v>0.2958191</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0.10344827600000001</v>
+      </c>
+      <c r="AG26">
+        <v>0.37931034499999999</v>
+      </c>
+      <c r="AH26">
+        <v>0.44827586200000002</v>
+      </c>
+      <c r="AI26">
+        <v>6.8965517000000004E-2</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27">
+        <v>0.61538461499999997</v>
+      </c>
+      <c r="C27">
+        <v>9.4069420000000001E-2</v>
+      </c>
+      <c r="D27">
+        <v>2.9476168330000001</v>
+      </c>
+      <c r="E27">
+        <v>4.1209780110000001</v>
+      </c>
+      <c r="F27">
+        <v>2.6666667000000002E-2</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1.7730769230000001</v>
+      </c>
+      <c r="J27">
+        <v>2.0310199930000001</v>
+      </c>
+      <c r="K27">
+        <v>0.64736411400000005</v>
+      </c>
+      <c r="L27">
+        <v>0.26923272599999998</v>
+      </c>
+      <c r="M27">
+        <v>1.7483171040000001</v>
+      </c>
+      <c r="N27">
+        <v>0.87750304999999995</v>
+      </c>
+      <c r="O27">
+        <v>0.32179667899999997</v>
+      </c>
+      <c r="P27">
+        <v>2.3200126000000001E-2</v>
+      </c>
+      <c r="Q27">
+        <v>5.1282050000000003E-3</v>
+      </c>
+      <c r="R27">
+        <v>3.0117284230000001</v>
+      </c>
+      <c r="S27">
+        <v>4.1913466430000001</v>
+      </c>
+      <c r="T27">
+        <v>9.0502816999999999E-2</v>
+      </c>
+      <c r="U27">
+        <v>3.3066919E-2</v>
+      </c>
+      <c r="V27">
+        <v>3.0769230000000001E-3</v>
+      </c>
+      <c r="W27">
+        <v>3.6384615380000001</v>
+      </c>
+      <c r="X27">
+        <v>1.613251303</v>
+      </c>
+      <c r="Y27">
+        <v>0.57888994000000005</v>
+      </c>
+      <c r="Z27">
+        <v>0.81958717999999997</v>
+      </c>
+      <c r="AA27">
+        <v>1.9735370759999999</v>
+      </c>
+      <c r="AB27">
+        <v>0.62245712900000005</v>
+      </c>
+      <c r="AC27">
+        <v>0.41573421799999999</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>7.6923077000000006E-2</v>
+      </c>
+      <c r="AG27">
+        <v>0.61538461499999997</v>
+      </c>
+      <c r="AH27">
+        <v>0.23076923099999999</v>
+      </c>
+      <c r="AI27">
+        <v>7.6923077000000006E-2</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="C28">
+        <v>1.6666669999999999E-3</v>
+      </c>
+      <c r="D28">
+        <v>2.8349913739999999</v>
+      </c>
+      <c r="E28">
+        <v>5.232791594</v>
+      </c>
+      <c r="F28">
+        <v>0.20643504300000001</v>
+      </c>
+      <c r="G28">
+        <v>0.102516711</v>
+      </c>
+      <c r="H28">
+        <v>4.5841359999999999E-3</v>
+      </c>
+      <c r="I28">
+        <v>6.3383333329999996</v>
+      </c>
+      <c r="J28">
+        <v>2.2351856859999999</v>
+      </c>
+      <c r="K28">
+        <v>0.27589508299999999</v>
+      </c>
+      <c r="L28">
+        <v>0.32391060500000002</v>
+      </c>
+      <c r="M28">
+        <v>0.838265064</v>
+      </c>
+      <c r="N28">
+        <v>0.82081370300000001</v>
+      </c>
+      <c r="O28">
+        <v>1.1759126070000001</v>
+      </c>
+      <c r="P28">
+        <v>9.8219724999999994E-2</v>
+      </c>
+      <c r="Q28">
+        <v>4.8267353999999998E-2</v>
+      </c>
+      <c r="R28">
+        <v>1.605594255</v>
+      </c>
+      <c r="S28">
+        <v>2.9052988389999999</v>
+      </c>
+      <c r="T28">
+        <v>3.6416713000000003E-2</v>
+      </c>
+      <c r="U28">
+        <v>2.6560706E-2</v>
+      </c>
+      <c r="V28">
+        <v>8.8493630000000007E-3</v>
+      </c>
+      <c r="W28">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="X28">
+        <v>1.179741699</v>
+      </c>
+      <c r="Y28">
+        <v>0.22855549</v>
+      </c>
+      <c r="Z28">
+        <v>0.19729706599999999</v>
+      </c>
+      <c r="AA28">
+        <v>0.87128849200000003</v>
+      </c>
+      <c r="AB28">
+        <v>0.34925753599999998</v>
+      </c>
+      <c r="AC28">
+        <v>0.38504822700000002</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <v>0.20833333300000001</v>
+      </c>
+      <c r="AH28">
+        <v>0.5</v>
+      </c>
+      <c r="AI28">
+        <v>0.16666666699999999</v>
+      </c>
+      <c r="AJ28">
+        <v>8.3333332999999996E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>0.63636363600000001</v>
+      </c>
+      <c r="C29">
+        <v>2.0147871000000001E-2</v>
+      </c>
+      <c r="D29">
+        <v>2.3335402940000001</v>
+      </c>
+      <c r="E29">
+        <v>3.379676914</v>
+      </c>
+      <c r="F29">
+        <v>0.186268512</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1.818182E-3</v>
+      </c>
+      <c r="I29">
+        <v>3.5484848480000002</v>
+      </c>
+      <c r="J29">
+        <v>1.9260453280000001</v>
+      </c>
+      <c r="K29">
+        <v>0.28120505099999998</v>
+      </c>
+      <c r="L29">
+        <v>0.126289915</v>
+      </c>
+      <c r="M29">
+        <v>1.198510999</v>
+      </c>
+      <c r="N29">
+        <v>0.46756720699999998</v>
+      </c>
+      <c r="O29">
+        <v>0.66746208799999995</v>
+      </c>
+      <c r="P29">
+        <v>9.5728615000000003E-2</v>
+      </c>
+      <c r="Q29">
+        <v>9.4976964999999997E-2</v>
+      </c>
+      <c r="R29">
+        <v>2.5289077</v>
+      </c>
+      <c r="S29">
+        <v>3.42694645</v>
+      </c>
+      <c r="T29">
+        <v>4.0147409000000002E-2</v>
+      </c>
+      <c r="U29">
+        <v>3.8300635E-2</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0.52651515199999999</v>
+      </c>
+      <c r="X29">
+        <v>1.650624208</v>
+      </c>
+      <c r="Y29">
+        <v>0.50799220300000003</v>
+      </c>
+      <c r="Z29">
+        <v>0.37029129</v>
+      </c>
+      <c r="AA29">
+        <v>1.6198460560000001</v>
+      </c>
+      <c r="AB29">
+        <v>0.69390512599999998</v>
+      </c>
+      <c r="AC29">
+        <v>0.21515651899999999</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>4.5454544999999999E-2</v>
+      </c>
+      <c r="AF29">
+        <v>0.27272727299999999</v>
+      </c>
+      <c r="AG29">
+        <v>0.27272727299999999</v>
+      </c>
+      <c r="AH29">
+        <v>0.409090909</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>0.69230769199999997</v>
+      </c>
+      <c r="C30">
+        <v>6.7084079999999999E-3</v>
+      </c>
+      <c r="D30">
+        <v>3.9443528269999999</v>
+      </c>
+      <c r="E30">
+        <v>5.0524637910000001</v>
+      </c>
+      <c r="F30">
+        <v>0.144431476</v>
+      </c>
+      <c r="G30">
+        <v>7.9148105999999996E-2</v>
+      </c>
+      <c r="H30">
+        <v>5.1684039999999997E-3</v>
+      </c>
+      <c r="I30">
+        <v>2.2205128209999998</v>
+      </c>
+      <c r="J30">
+        <v>3.0429103949999998</v>
+      </c>
+      <c r="K30">
+        <v>0.63240750000000001</v>
+      </c>
+      <c r="L30">
+        <v>0.269034932</v>
+      </c>
+      <c r="M30">
+        <v>2.6090848900000001</v>
+      </c>
+      <c r="N30">
+        <v>0.26454408899999998</v>
+      </c>
+      <c r="O30">
+        <v>1.0707238480000001</v>
+      </c>
+      <c r="P30">
+        <v>1.7036536000000001E-2</v>
+      </c>
+      <c r="Q30">
+        <v>8.7912089999999995E-3</v>
+      </c>
+      <c r="R30">
+        <v>2.4489341439999999</v>
+      </c>
+      <c r="S30">
+        <v>4.390230517</v>
+      </c>
+      <c r="T30">
+        <v>5.4832346999999997E-2</v>
+      </c>
+      <c r="U30">
+        <v>5.1684039999999997E-3</v>
+      </c>
+      <c r="V30">
+        <v>1.0296609E-2</v>
+      </c>
+      <c r="W30">
+        <v>1.597435897</v>
+      </c>
+      <c r="X30">
+        <v>1.4909417549999999</v>
+      </c>
+      <c r="Y30">
+        <v>0.36062211199999999</v>
+      </c>
+      <c r="Z30">
+        <v>0.59737027700000001</v>
+      </c>
+      <c r="AA30">
+        <v>1.7433928379999999</v>
+      </c>
+      <c r="AB30">
+        <v>0.32211435999999999</v>
+      </c>
+      <c r="AC30">
+        <v>0.38342694700000002</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>7.6923077000000006E-2</v>
+      </c>
+      <c r="AG30">
+        <v>0.46153846199999998</v>
+      </c>
+      <c r="AH30">
+        <v>0.38461538499999998</v>
+      </c>
+      <c r="AI30">
+        <v>7.6923077000000006E-2</v>
+      </c>
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31">
+        <v>0.91666666699999999</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.81994810799999995</v>
+      </c>
+      <c r="E31">
+        <v>6.1059657400000003</v>
+      </c>
+      <c r="F31">
+        <v>0.24225675399999999</v>
+      </c>
+      <c r="G31">
+        <v>0.39930052199999999</v>
+      </c>
+      <c r="H31">
+        <v>0.18020330700000001</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0.47533125300000001</v>
+      </c>
+      <c r="K31">
+        <v>0.12469113900000001</v>
+      </c>
+      <c r="L31">
+        <v>0.21992571599999999</v>
+      </c>
+      <c r="M31">
+        <v>0.15219374899999999</v>
+      </c>
+      <c r="N31">
+        <v>0.27203381300000001</v>
+      </c>
+      <c r="O31">
+        <v>0.39572054600000001</v>
+      </c>
+      <c r="P31">
+        <v>1.7921146999999998E-2</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0.87662078099999996</v>
+      </c>
+      <c r="S31">
+        <v>1.277974001</v>
+      </c>
+      <c r="T31">
+        <v>0.115936129</v>
+      </c>
+      <c r="U31">
+        <v>1.7921146999999998E-2</v>
+      </c>
+      <c r="V31">
+        <v>1.7857142999999999E-2</v>
+      </c>
+      <c r="W31">
+        <v>3.4333333330000002</v>
+      </c>
+      <c r="X31">
+        <v>0.56384257699999996</v>
+      </c>
+      <c r="Y31">
+        <v>0.25907876699999999</v>
+      </c>
+      <c r="Z31">
+        <v>5.3699437000000003E-2</v>
+      </c>
+      <c r="AA31">
+        <v>6.8823681999999997E-2</v>
+      </c>
+      <c r="AB31">
+        <v>0.16654812199999999</v>
+      </c>
+      <c r="AC31">
+        <v>0.64124897700000005</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>0.16666666699999999</v>
+      </c>
+      <c r="AI31">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AJ31">
         <v>0</v>
       </c>
     </row>

</xml_diff>